<commit_message>
Updates to ODH to use US Core
</commit_message>
<xml_diff>
--- a/docs/odh/obf-Appointment.xlsx
+++ b/docs/odh/obf-Appointment.xlsx
@@ -651,7 +651,7 @@
     <t>Appointment.supportingInformation</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/odh/StructureDefinition/obf-DomainResource)
+    <t xml:space="preserve">Reference(Resource)
 </t>
   </si>
   <si>
@@ -824,7 +824,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/odh/StructureDefinition/obf-ReferralRequest)
+    <t xml:space="preserve">Reference(ServiceRequest)
 </t>
   </si>
   <si>
@@ -938,7 +938,7 @@
     <t>Appointment.participant.actor</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/odh/StructureDefinition/obf-Patient|http://hl7.org/fhir/us/odh/StructureDefinition/obf-Practitioner|http://hl7.org/fhir/us/odh/StructureDefinition/obf-RelatedPerson|http://hl7.org/fhir/us/odh/StructureDefinition/obf-Device|http://hl7.org/fhir/us/odh/StructureDefinition/obf-Location)
+    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient|http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitioner|RelatedPerson|http://hl7.org/fhir/us/core/StructureDefinition/us-core-device|http://hl7.org/fhir/us/core/StructureDefinition/us-core-location)
 </t>
   </si>
   <si>

</xml_diff>